<commit_message>
add corrected input file
</commit_message>
<xml_diff>
--- a/data/Fall2018/db1-7_all-timepoints-runs/db1/16-genes_36-edges_db1_Sigmoid_estimation_all-timepoints.xlsx
+++ b/data/Fall2018/db1-7_all-timepoints-runs/db1/16-genes_36-edges_db1_Sigmoid_estimation_all-timepoints.xlsx
@@ -2208,7 +2208,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2218,7 +2218,7 @@
     <col min="2" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -2335,8 +2335,14 @@
       <c r="D14" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E14" s="1">
+        <v>90</v>
+      </c>
+      <c r="F14" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -2359,7 +2365,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -2401,6 +2407,42 @@
       </c>
       <c r="N16" s="1">
         <v>60</v>
+      </c>
+      <c r="O16" s="1">
+        <v>65</v>
+      </c>
+      <c r="P16" s="1">
+        <v>70</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>75</v>
+      </c>
+      <c r="R16" s="1">
+        <v>80</v>
+      </c>
+      <c r="S16" s="1">
+        <v>85</v>
+      </c>
+      <c r="T16" s="1">
+        <v>90</v>
+      </c>
+      <c r="U16" s="1">
+        <v>95</v>
+      </c>
+      <c r="V16" s="1">
+        <v>100</v>
+      </c>
+      <c r="W16" s="1">
+        <v>105</v>
+      </c>
+      <c r="X16" s="1">
+        <v>110</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>115</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>